<commit_message>
Update file paths and graph output filename
</commit_message>
<xml_diff>
--- a/Book3.xlsx
+++ b/Book3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyow\dev\chime-KPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\user\workspace\chimeKPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C4C434-10AC-446A-8524-DE3AB0EEC4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887D886F-A220-4627-A5FB-8529FD5E1DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="21600" windowHeight="12670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32790" yWindow="5565" windowWidth="15765" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,37 +133,37 @@
       <sheetData sheetId="3">
         <row r="1">
           <cell r="A1">
-            <v>13</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="2">
           <cell r="A2">
-            <v>13</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3">
-            <v>13</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4">
-            <v>13</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5">
-            <v>13</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6">
-            <v>13</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7">
-            <v>13</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="8">
@@ -540,9 +540,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,10 +553,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
         <f>[1]Sheet1!$A1</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -565,10 +565,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
         <f>[1]Sheet1!$A2</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -577,10 +577,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
         <f>[1]Sheet1!$A3</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -589,10 +589,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
         <f>[1]Sheet1!$A4</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -601,10 +601,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
         <f>[1]Sheet1!$A5</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -613,10 +613,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
         <f>[1]Sheet1!$A6</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -625,10 +625,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
         <f>[1]Sheet1!$A7</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -637,7 +637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
         <f>[1]Sheet1!$A8</f>
         <v>13</v>
@@ -649,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
         <f>[1]Sheet1!$A9</f>
         <v>13</v>
@@ -661,7 +661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
         <f>[1]Sheet1!$A10</f>
         <v>13</v>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
         <f>[1]Sheet1!$A11</f>
         <v>13</v>
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13">
         <f>[1]Sheet1!$A12</f>
         <v>13</v>
@@ -697,7 +697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14">
         <f>[1]Sheet1!$A13</f>
         <v>13</v>
@@ -709,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15">
         <f>[1]Sheet1!$A14</f>
         <v>13</v>
@@ -721,7 +721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16">
         <f>[1]Sheet1!$A15</f>
         <v>13</v>
@@ -733,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17">
         <f>[1]Sheet1!$A16</f>
         <v>13</v>
@@ -745,7 +745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18">
         <f>[1]Sheet1!$A17</f>
         <v>0</v>
@@ -757,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19">
         <f>[1]Sheet1!$A18</f>
         <v>0</v>
@@ -769,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20">
         <f>[1]Sheet1!$A19</f>
         <v>0</v>
@@ -781,7 +781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21">
         <f>[1]Sheet1!$A20</f>
         <v>0</v>
@@ -793,7 +793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22">
         <f>[1]Sheet1!$A21</f>
         <v>0</v>
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23">
         <f>[1]Sheet1!$A22</f>
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24">
         <f>[1]Sheet1!$A23</f>
         <v>0</v>
@@ -829,7 +829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25">
         <f>[1]Sheet1!$A24</f>
         <v>0</v>
@@ -841,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26">
         <f>[1]Sheet1!$A25</f>
         <v>0</v>
@@ -853,7 +853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27">
         <f>[1]Sheet1!$A26</f>
         <v>0</v>
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28">
         <f>[1]Sheet1!$A27</f>
         <v>0</v>
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29">
         <f>[1]Sheet1!$A28</f>
         <v>0</v>
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30">
         <f>[1]Sheet1!$A29</f>
         <v>0</v>
@@ -901,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31">
         <f>[1]Sheet1!$A30</f>
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32">
         <f>[1]Sheet1!$A31</f>
         <v>0</v>
@@ -925,7 +925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33">
         <f>[1]Sheet1!$A32</f>
         <v>0</v>
@@ -937,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34">
         <f>[1]Sheet1!$A33</f>
         <v>0</v>
@@ -949,7 +949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35">
         <f>[1]Sheet1!$A34</f>
         <v>0</v>
@@ -961,7 +961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36">
         <f>[1]Sheet1!$A35</f>
         <v>0</v>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37">
         <f>[1]Sheet1!$A36</f>
         <v>0</v>
@@ -985,7 +985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38">
         <f>[1]Sheet1!$A37</f>
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39">
         <f>[1]Sheet1!$A38</f>
         <v>0</v>

</xml_diff>